<commit_message>
Fix test 23 on the Advanced Alerts Test sheet in the demo
CSV wasn't attached, now it is.
</commit_message>
<xml_diff>
--- a/demo/tests.xlsx
+++ b/demo/tests.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcoles\Documents\GitHub\VizAlerts\demo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="19275" windowHeight="11970" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="19275" windowHeight="11970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Alerts" sheetId="5" r:id="rId1"/>
@@ -12,12 +17,12 @@
     <sheet name="Other Tests" sheetId="2" r:id="rId3"/>
     <sheet name="Map Category to Manager" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="138">
   <si>
     <t xml:space="preserve"> Email Action *</t>
   </si>
@@ -182,9 +187,6 @@
   </si>
   <si>
     <t>VIZ_PDF(VizAlertsDemo/Overview?Region=East|filename=EastSales|mergepdf) VIZ_PDF(VizAlertsDemo/Product?Region=East|filename=EastSales|mergepdf)</t>
-  </si>
-  <si>
-    <t>VIZ_PDF(VizAlertsDemo/Overview?Region=East|filename=EastSales|mergepdf) VIZ_PDF(VizAlertsDemo/Product?Region=East|filename=EastSales|mergepdf) VIZ_PDF(VizAlertsDemo/Overview?Region=West|filename=WestSales|mergepdf) VIZ_PDF(VizAlertsDemo/Product?Region=West|filename=WestSales|mergepdf)</t>
   </si>
   <si>
     <t>Some body text&lt;br/&gt;</t>
@@ -493,6 +495,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -540,7 +545,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -575,7 +580,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -797,27 +802,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -829,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,7 +858,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1033,7 +1038,7 @@
         <v>Test 7: VIZ_IMAGE() in footer</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
@@ -1101,7 +1106,7 @@
         <v>Test 10: VIZ_IMAGE() w/custom size</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1116,14 +1121,14 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Test 11: VIZ_IMAGE() w/link to image</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="E12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Test 11: VIZ_IMAGE() w/link to image</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1138,14 +1143,14 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Test 12: VIZ_LINK() in body</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="E13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Test 12: VIZ_LINK() in body</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1160,14 +1165,14 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Test 13: VIZ_LINK() w/custom workbook/viewname</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="E14" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Test 13: VIZ_LINK() w/custom workbook/viewname</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1182,14 +1187,14 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Test 14: VIZ_LINK() w/custom workbook/viewname and custom text</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="E15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Test 14: VIZ_LINK() w/custom workbook/viewname and custom text</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1204,14 +1209,14 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Test 15: VIZ_LINK() w/raw link</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="E16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Test 15: VIZ_LINK() w/raw link</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1395,12 +1400,12 @@
         <v>Test 23: Merge PDFs to multiple output PDFs within single VizAlerts row</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1412,21 +1417,21 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E25" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 24: Advanced Alert Demo</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1448,7 +1453,7 @@
         <v>Test 25: Consolidate emails w/no extras</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1474,7 +1479,7 @@
         <v>Test 25: Consolidate emails w/no extras</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1500,7 +1505,7 @@
         <v>Test 25: Consolidate emails w/no extras</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -1553,7 +1558,7 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -1579,7 +1584,7 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -1606,7 +1611,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1632,7 +1637,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1727,14 +1732,14 @@
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E37" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 29: Consolidate email w/multiple attachments</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -1755,7 +1760,7 @@
         <v>2</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E38" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1765,7 +1770,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J38" s="1"/>
     </row>
@@ -1781,7 +1786,7 @@
         <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E39" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1791,7 +1796,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J39" s="1"/>
     </row>
@@ -1814,12 +1819,12 @@
         <v>Test 30: Consolidate email w/merged PDFs</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J40" s="1"/>
     </row>
@@ -1845,7 +1850,7 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J41" s="1"/>
     </row>
@@ -1871,7 +1876,7 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J42" s="1"/>
     </row>
@@ -1887,19 +1892,19 @@
         <v>1</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E43" s="1" t="str">
         <f>"Test " &amp; B43 &amp; ": " &amp; D43</f>
         <v>Test 31: Consolidate email w/merged PDFs and other attachment</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J43" s="1"/>
     </row>
@@ -1915,7 +1920,7 @@
         <v>2</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E44" s="1" t="str">
         <f t="shared" ref="E44:E45" si="3">"Test " &amp; B44 &amp; ": " &amp; D44</f>
@@ -1925,7 +1930,7 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J44" s="1"/>
     </row>
@@ -1941,7 +1946,7 @@
         <v>3</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E45" s="1" t="str">
         <f t="shared" si="3"/>
@@ -1951,7 +1956,7 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J45" s="1"/>
     </row>
@@ -1971,9 +1976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2001,7 +2004,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2012,14 +2015,14 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D16" si="0">"Test " &amp; B2 &amp; ": " &amp; C2</f>
         <v>Test 1: Incomplete viz reference: expect failure to download</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2030,14 +2033,14 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
         <v>Test 2: Content reference that accesses hidden worksheet: expect failure to download</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2048,14 +2051,14 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
         <v>Test 3: Content reference for non-existent worksheet: expect failure to download</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2066,14 +2069,14 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
         <v>Test 4: Content reference with no workbookview, only URL parameter: expect filtered trigger viz</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2084,14 +2087,14 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>Test 5: Content reference w/ no workbookview, only filename: expect trigger viz w/filename</v>
       </c>
       <c r="F6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2102,14 +2105,14 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
         <v>Test 6: Content reference w/ no workbookview, only non-existent | argument: expect trigger viz</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2120,14 +2123,14 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
         <v>Test 7: Using pipe character '|' inside URL parameter: generates unexpected results (no East filter)</v>
       </c>
       <c r="E8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2138,14 +2141,14 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
         <v>Test 8: Content reference inside content reference: expect failure to download</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2156,14 +2159,14 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
         <v>Test 9: URL Parameter with space: expect viz to render</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2174,14 +2177,14 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
         <v>Test 10: Filename with space: expect viz with spaces in filename</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2192,14 +2195,14 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
         <v>Test 11: Illegal filename with \: expect error</v>
       </c>
       <c r="F12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2210,14 +2213,14 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
         <v>Test 12: Illegal filename with ..\: expect error</v>
       </c>
       <c r="F13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2228,14 +2231,14 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
         <v>Test 13: Illegal filename with absolute reference: expect error</v>
       </c>
       <c r="F14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2246,14 +2249,14 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
         <v>Test 14: Content reference with filter that generates blank view: expect blank view</v>
       </c>
       <c r="E15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2264,14 +2267,14 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
         <v>Test 15: Illegal filename with &gt;: expect error</v>
       </c>
       <c r="F16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2299,13 +2302,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -2316,13 +2319,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D2" t="str">
         <f>B2 &amp;", you have a Low Margin Warning"</f>
@@ -2335,13 +2338,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D4" si="0">B3 &amp;", you have a Low Margin Warning"</f>
@@ -2354,13 +2357,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Final documentation changes by jdrummey
</commit_message>
<xml_diff>
--- a/demo/tests.xlsx
+++ b/demo/tests.xlsx
@@ -1,47 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcoles\Documents\GitHub\VizAlerts\demo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="19275" windowHeight="11970" activeTab="1"/>
+    <workbookView xWindow="1440" yWindow="2880" windowWidth="19280" windowHeight="11980" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Alerts" sheetId="5" r:id="rId1"/>
     <sheet name="Advanced Alerts" sheetId="1" r:id="rId2"/>
     <sheet name="Other Tests" sheetId="2" r:id="rId3"/>
     <sheet name="Map Category to Manager" sheetId="7" r:id="rId4"/>
+    <sheet name="SMS Tests" sheetId="8" r:id="rId5"/>
+    <sheet name="SMS Other Tests" sheetId="9" r:id="rId6"/>
+    <sheet name="Excel Number Tests" sheetId="10" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="177">
   <si>
     <t xml:space="preserve"> Email Action *</t>
   </si>
   <si>
-    <t xml:space="preserve"> Email Subject *</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Email Body *</t>
   </si>
   <si>
-    <t xml:space="preserve"> Email Header ~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Email Footer ~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Email Consolidate ~</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
@@ -117,9 +108,6 @@
     <t>Body and CSV attachment</t>
   </si>
   <si>
-    <t>Email Attachment ~</t>
-  </si>
-  <si>
     <t>This email should have this text and a CSV attachment</t>
   </si>
   <si>
@@ -189,6 +177,9 @@
     <t>VIZ_PDF(VizAlertsDemo/Overview?Region=East|filename=EastSales|mergepdf) VIZ_PDF(VizAlertsDemo/Product?Region=East|filename=EastSales|mergepdf)</t>
   </si>
   <si>
+    <t>VIZ_PDF(VizAlertsDemo/Overview?Region=East|filename=EastSales|mergepdf) VIZ_PDF(VizAlertsDemo/Product?Region=East|filename=EastSales|mergepdf) VIZ_PDF(VizAlertsDemo/Overview?Region=West|filename=WestSales|mergepdf) VIZ_PDF(VizAlertsDemo/Product?Region=West|filename=WestSales|mergepdf)</t>
+  </si>
+  <si>
     <t>Some body text&lt;br/&gt;</t>
   </si>
   <si>
@@ -249,9 +240,6 @@
     <t>Should *not* see this footer from 2nd row</t>
   </si>
   <si>
-    <t xml:space="preserve"> Email Attachment ~</t>
-  </si>
-  <si>
     <t>VIZ_IMAGE(VizAlertsDemo)</t>
   </si>
   <si>
@@ -429,20 +417,152 @@
     <t>jonathan@datablick.com</t>
   </si>
   <si>
-    <t xml:space="preserve"> Email To *</t>
-  </si>
-  <si>
     <t>Illegal filename with &gt;: expect error</t>
   </si>
   <si>
     <t>VIZ_CSV(|filename=foo&gt;bar)</t>
+  </si>
+  <si>
+    <t>test for 2 numbers</t>
+  </si>
+  <si>
+    <t>number in x.xxx.xxx.xxxx format</t>
+  </si>
+  <si>
+    <t>number in +x (xxx) xxx-xxxx format</t>
+  </si>
+  <si>
+    <t>header in SMS</t>
+  </si>
+  <si>
+    <t>should see a header</t>
+  </si>
+  <si>
+    <t>footer in SMS</t>
+  </si>
+  <si>
+    <t>should see a footer</t>
+  </si>
+  <si>
+    <t>header and footer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">should see a footer </t>
+  </si>
+  <si>
+    <t>VIZ_LINK() alert</t>
+  </si>
+  <si>
+    <t>SMS Action</t>
+  </si>
+  <si>
+    <t>Email Subject</t>
+  </si>
+  <si>
+    <t>Email Body</t>
+  </si>
+  <si>
+    <t>Email Header</t>
+  </si>
+  <si>
+    <t>Email Footer</t>
+  </si>
+  <si>
+    <t>Email Attachment</t>
+  </si>
+  <si>
+    <t>Email Consolidate</t>
+  </si>
+  <si>
+    <t>Email Action</t>
+  </si>
+  <si>
+    <t>Email To</t>
+  </si>
+  <si>
+    <t>SMS Message</t>
+  </si>
+  <si>
+    <t>simple test</t>
+  </si>
+  <si>
+    <t>1st row&lt;br/&gt;</t>
+  </si>
+  <si>
+    <t>Consolidate 3 rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nd row&lt;br/&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3rd row&lt;br/&gt; </t>
+  </si>
+  <si>
+    <t>SMS Header</t>
+  </si>
+  <si>
+    <t>SMS Footer</t>
+  </si>
+  <si>
+    <t>http://github.com/tableau/VizAlerts alert in body</t>
+  </si>
+  <si>
+    <t>Expected Test Result</t>
+  </si>
+  <si>
+    <t>no subject &amp; no body</t>
+  </si>
+  <si>
+    <t>failure due to 0 length</t>
+  </si>
+  <si>
+    <t>number too short</t>
+  </si>
+  <si>
+    <t>expect failure</t>
+  </si>
+  <si>
+    <t>email address in number</t>
+  </si>
+  <si>
+    <t>bad number</t>
+  </si>
+  <si>
+    <t>text and numbers mixed</t>
+  </si>
+  <si>
+    <t>SMS w/raw HTML</t>
+  </si>
+  <si>
+    <t>default footer w/raw HTML</t>
+  </si>
+  <si>
+    <t>VIZALERTS_FOOTER()</t>
+  </si>
+  <si>
+    <t>no number - empty SMS To</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;HTML&lt;/b&gt; in body</t>
+  </si>
+  <si>
+    <t>number is raw number</t>
+  </si>
+  <si>
+    <t>number is text</t>
+  </si>
+  <si>
+    <t>12078319657</t>
+  </si>
+  <si>
+    <t>SMS To</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,6 +574,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -476,16 +604,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -494,9 +641,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -545,7 +689,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -580,7 +724,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -795,38 +939,43 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -834,55 +983,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>144</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>4</v>
+        <v>146</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>31</v>
+        <v>147</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -891,20 +1040,20 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="str">
         <f>"Test " &amp; B2 &amp; ": " &amp; D2</f>
         <v>Test 1: Advanced Alert w/no extras</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -913,22 +1062,22 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="str">
         <f>"Test " &amp; B3 &amp; ": " &amp; D3</f>
         <v>Test 2: Custom Header</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -937,22 +1086,22 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" ref="E4:E5" si="0">"Test " &amp; B4 &amp; ": " &amp; D4</f>
         <v>Test 3: Custom Footer w/out Default Footer</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -961,22 +1110,22 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Test 4: Custom Footer</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -985,20 +1134,20 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" ref="E6:E39" si="1">"Test " &amp; B6 &amp; ": " &amp; D6</f>
         <v>Test 5: VIZ_IMAGE() in body</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1007,22 +1156,22 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 6: VIZ_IMAGE() in header</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1031,22 +1180,22 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 7: VIZ_IMAGE() in footer</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1055,20 +1204,20 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E9" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 8: VIZ_IMAGE() w/custom workbook/view</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1077,20 +1226,20 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 9: VIZ_IMAGE() w/custom URL parameter</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1099,20 +1248,20 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 10: VIZ_IMAGE() w/custom size</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -1121,20 +1270,20 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E12" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 11: VIZ_IMAGE() w/link to image</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1143,20 +1292,20 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E13" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 12: VIZ_LINK() in body</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1165,20 +1314,20 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E14" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 13: VIZ_LINK() w/custom workbook/viewname</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1187,20 +1336,20 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E15" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 14: VIZ_LINK() w/custom workbook/viewname and custom text</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -1209,20 +1358,20 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E16" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 15: VIZ_LINK() w/raw link</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1231,20 +1380,20 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E17" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 16: Multiple vizzes in body</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -1253,22 +1402,22 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E18" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 17: Body and CSV attachment</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -1277,7 +1426,7 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E19" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1287,10 +1436,10 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -1299,22 +1448,22 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E20" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 19: Body and PDF attachment</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1323,22 +1472,22 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E21" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 20: Multiple attachments</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -1347,7 +1496,7 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E22" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1357,10 +1506,10 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -1369,22 +1518,22 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E23" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 22: Merge PDFs within single VizAlerts row</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -1393,22 +1542,22 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E24" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 23: Merge PDFs to multiple output PDFs within single VizAlerts row</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -1417,24 +1566,24 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E25" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 24: Advanced Alert Demo</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -1446,21 +1595,21 @@
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E26" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 25: Consolidate emails w/no extras</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -1472,21 +1621,21 @@
         <v>2</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E27" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 25: Consolidate emails w/no extras</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -1498,21 +1647,21 @@
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E28" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 25: Consolidate emails w/no extras</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -1524,7 +1673,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E29" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1532,13 +1681,13 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -1550,7 +1699,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E30" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1558,13 +1707,13 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -1576,7 +1725,7 @@
         <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E31" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1584,13 +1733,13 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -1602,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E32" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1611,12 +1760,12 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>1</v>
       </c>
@@ -1628,7 +1777,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E33" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1637,12 +1786,12 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>1</v>
       </c>
@@ -1654,7 +1803,7 @@
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E34" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1663,12 +1812,12 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -1680,21 +1829,21 @@
         <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E35" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 28: Consolidated emails w/ multiple VIZ_IMAGEs</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -1706,21 +1855,21 @@
         <v>2</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E36" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 28: Consolidated emails w/ multiple VIZ_IMAGEs</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>1</v>
       </c>
@@ -1732,23 +1881,23 @@
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E37" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Test 29: Consolidate email w/multiple attachments</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>1</v>
       </c>
@@ -1760,7 +1909,7 @@
         <v>2</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E38" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1770,11 +1919,11 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>1</v>
       </c>
@@ -1786,7 +1935,7 @@
         <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E39" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1796,11 +1945,11 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>1</v>
       </c>
@@ -1812,23 +1961,23 @@
         <v>1</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E40" s="1" t="str">
         <f>"Test " &amp; B40 &amp; ": " &amp; D40</f>
         <v>Test 30: Consolidate email w/merged PDFs</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -1840,7 +1989,7 @@
         <v>2</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E41" s="1" t="str">
         <f>"Test " &amp; B41 &amp; ": " &amp; D41</f>
@@ -1850,11 +1999,11 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>1</v>
       </c>
@@ -1866,7 +2015,7 @@
         <v>3</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E42" s="1" t="str">
         <f t="shared" ref="E42" si="2">"Test " &amp; B42 &amp; ": " &amp; D42</f>
@@ -1876,11 +2025,11 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>1</v>
       </c>
@@ -1892,23 +2041,23 @@
         <v>1</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E43" s="1" t="str">
         <f>"Test " &amp; B43 &amp; ": " &amp; D43</f>
         <v>Test 31: Consolidate email w/merged PDFs and other attachment</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>1</v>
       </c>
@@ -1920,7 +2069,7 @@
         <v>2</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E44" s="1" t="str">
         <f t="shared" ref="E44:E45" si="3">"Test " &amp; B44 &amp; ": " &amp; D44</f>
@@ -1930,11 +2079,11 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>1</v>
       </c>
@@ -1946,7 +2095,7 @@
         <v>3</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E45" s="1" t="str">
         <f t="shared" si="3"/>
@@ -1956,11 +2105,11 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -1969,6 +2118,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1976,38 +2130,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.1640625" customWidth="1"/>
+    <col min="5" max="5" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>144</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2015,17 +2171,17 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D16" si="0">"Test " &amp; B2 &amp; ": " &amp; C2</f>
         <v>Test 1: Incomplete viz reference: expect failure to download</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2033,17 +2189,17 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
         <v>Test 2: Content reference that accesses hidden worksheet: expect failure to download</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2051,17 +2207,17 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
         <v>Test 3: Content reference for non-existent worksheet: expect failure to download</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2069,17 +2225,17 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
         <v>Test 4: Content reference with no workbookview, only URL parameter: expect filtered trigger viz</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2087,17 +2243,17 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>Test 5: Content reference w/ no workbookview, only filename: expect trigger viz w/filename</v>
       </c>
       <c r="F6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2105,17 +2261,17 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
         <v>Test 6: Content reference w/ no workbookview, only non-existent | argument: expect trigger viz</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2123,17 +2279,17 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
         <v>Test 7: Using pipe character '|' inside URL parameter: generates unexpected results (no East filter)</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2141,17 +2297,17 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
         <v>Test 8: Content reference inside content reference: expect failure to download</v>
       </c>
       <c r="E9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2159,17 +2315,17 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
         <v>Test 9: URL Parameter with space: expect viz to render</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2177,17 +2333,17 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
         <v>Test 10: Filename with space: expect viz with spaces in filename</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2195,17 +2351,17 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
         <v>Test 11: Illegal filename with \: expect error</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2213,17 +2369,17 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
         <v>Test 12: Illegal filename with ..\: expect error</v>
       </c>
       <c r="F13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2231,17 +2387,17 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
         <v>Test 13: Illegal filename with absolute reference: expect error</v>
       </c>
       <c r="F14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2249,17 +2405,17 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
         <v>Test 14: Content reference with filter that generates blank view: expect blank view</v>
       </c>
       <c r="E15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2267,14 +2423,14 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
         <v>Test 15: Illegal filename with &gt;: expect error</v>
       </c>
       <c r="F16" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2282,6 +2438,11 @@
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2290,42 +2451,42 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="C1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="D2" t="str">
         <f>B2 &amp;", you have a Low Margin Warning"</f>
@@ -2336,15 +2497,15 @@
         <v>&lt;p&gt;Hello Alice,&lt;/p&gt;&lt;p&gt;You have a low margin warning, please take a look this week&lt;/p&gt;VIZ_IMAGE(VizAlertsDemo/LowMarginWarning?Category=Furniture&amp;:size=600,400|vizlink)</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D4" si="0">B3 &amp;", you have a Low Margin Warning"</f>
@@ -2355,15 +2516,15 @@
         <v>&lt;p&gt;Hello Bob,&lt;/p&gt;&lt;p&gt;You have a low margin warning, please take a look this week&lt;/p&gt;VIZ_IMAGE(VizAlertsDemo/LowMarginWarning?Category=Office Supplies&amp;:size=600,400|vizlink)</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -2381,5 +2542,519 @@
     <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f>"Test " &amp; B2 &amp; ": " &amp; C2</f>
+        <v>Test 1: simple test</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f>"Test " &amp; B3 &amp; ": " &amp; C3</f>
+        <v>Test 2: test for 2 numbers</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>"Test " &amp; B4 &amp; ": " &amp; C4</f>
+        <v>Test 3: number in x.xxx.xxx.xxxx format</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f>"Test " &amp; B5 &amp; ": " &amp; C5</f>
+        <v>Test 4: number in +x (xxx) xxx-xxxx format</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>"Test " &amp; B6 &amp; ": " &amp; C6</f>
+        <v>Test 5: header in SMS</v>
+      </c>
+      <c r="G6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f>"Test " &amp; B7 &amp; ": " &amp; C7</f>
+        <v>Test 6: footer in SMS</v>
+      </c>
+      <c r="H7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f>"Test " &amp; B8 &amp; ": " &amp; C8</f>
+        <v>Test 7: header and footer</v>
+      </c>
+      <c r="G8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f>"Test " &amp; B9 &amp; ": " &amp; C9</f>
+        <v>Test 8: http://github.com/tableau/VizAlerts alert in body</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f>"Test " &amp; B10 &amp; ": " &amp; C10</f>
+        <v>Test 9: VIZ_LINK() alert</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" t="str">
+        <f>"Test " &amp; B11 &amp; ": " &amp; C11</f>
+        <v>Test 10: Consolidate 3 rows</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="H2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f t="shared" ref="D3:D9" si="0">"Test " &amp; B3 &amp; ": " &amp; C3</f>
+        <v>Test 2: number too short</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Test 3: email address in number</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Test 4: bad number</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Test 5: no number - empty SMS To</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Test 6: text and numbers mixed</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Test 7: &lt;b&gt;HTML&lt;/b&gt; in body</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Test 8: default footer w/raw HTML</v>
+      </c>
+      <c r="G9" t="s">
+        <v>170</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f>"Test " &amp; B2 &amp; ": " &amp; C2</f>
+        <v>Test 1: number is raw number</v>
+      </c>
+      <c r="E2">
+        <v>12078319657</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f>"Test " &amp; B3 &amp; ": " &amp; C3</f>
+        <v>Test 1: number is text</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final changes to 2.0.1, I totally promise
just missed a tab and a test
</commit_message>
<xml_diff>
--- a/demo/tests.xlsx
+++ b/demo/tests.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcoles\Documents\GitHub\VizAlerts\demo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="2880" windowWidth="19280" windowHeight="11980" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="1440" yWindow="2880" windowWidth="19275" windowHeight="11985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Alerts" sheetId="5" r:id="rId1"/>
@@ -15,7 +20,7 @@
     <sheet name="SMS Other Tests" sheetId="9" r:id="rId6"/>
     <sheet name="Excel Number Tests" sheetId="10" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="180">
   <si>
     <t xml:space="preserve"> Email Action *</t>
   </si>
@@ -556,6 +561,15 @@
   </si>
   <si>
     <t>SMS To</t>
+  </si>
+  <si>
+    <t>Test 32: Multiple text links</t>
+  </si>
+  <si>
+    <t>Should see a link to the Advanced Alerts trigger view here: VIZ_LINK()&lt;br /&gt;Should see &lt;b&gt;another&lt;/b&gt; link to the Advanced Alerts trigger view here: VIZ_LINK()</t>
+  </si>
+  <si>
+    <t>Multiple text links</t>
   </si>
 </sst>
 </file>
@@ -641,6 +655,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -939,32 +956,32 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -983,23 +1000,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1046,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1053,7 +1068,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1077,7 +1092,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1101,7 +1116,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1125,7 +1140,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1147,7 +1162,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1171,7 +1186,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1195,7 +1210,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1217,7 +1232,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1239,7 +1254,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1261,7 +1276,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -1283,7 +1298,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1305,7 +1320,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1327,7 +1342,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1349,7 +1364,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -1371,7 +1386,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1393,7 +1408,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -1417,7 +1432,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -1439,7 +1454,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -1463,7 +1478,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1487,7 +1502,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -1509,7 +1524,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -1533,7 +1548,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -1557,7 +1572,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -1583,7 +1598,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -1609,7 +1624,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -1635,7 +1650,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -1661,7 +1676,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -1687,7 +1702,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -1713,7 +1728,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -1739,7 +1754,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -1765,7 +1780,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>1</v>
       </c>
@@ -1791,7 +1806,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>1</v>
       </c>
@@ -1817,7 +1832,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -1843,7 +1858,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -1869,7 +1884,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1</v>
       </c>
@@ -1897,7 +1912,7 @@
       </c>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1</v>
       </c>
@@ -1923,7 +1938,7 @@
       </c>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>1</v>
       </c>
@@ -1949,7 +1964,7 @@
       </c>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1</v>
       </c>
@@ -1977,7 +1992,7 @@
       </c>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -2003,7 +2018,7 @@
       </c>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>1</v>
       </c>
@@ -2029,7 +2044,7 @@
       </c>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>1</v>
       </c>
@@ -2057,7 +2072,7 @@
       </c>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>1</v>
       </c>
@@ -2083,7 +2098,7 @@
       </c>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>1</v>
       </c>
@@ -2109,9 +2124,25 @@
       </c>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10">
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>32</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -2134,16 +2165,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.1640625" customWidth="1"/>
-    <col min="5" max="5" width="38.1640625" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" customWidth="1"/>
+    <col min="5" max="5" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>149</v>
       </c>
@@ -2163,7 +2194,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2181,7 +2212,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2199,7 +2230,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2217,7 +2248,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2235,7 +2266,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2253,7 +2284,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2271,7 +2302,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2289,7 +2320,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2307,7 +2338,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2325,7 +2356,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2343,7 +2374,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2361,7 +2392,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2379,7 +2410,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2397,7 +2428,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2415,7 +2446,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2454,14 +2485,14 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="4" max="4" width="35.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>119</v>
       </c>
@@ -2478,7 +2509,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -2497,7 +2528,7 @@
         <v>&lt;p&gt;Hello Alice,&lt;/p&gt;&lt;p&gt;You have a low margin warning, please take a look this week&lt;/p&gt;VIZ_IMAGE(VizAlertsDemo/LowMarginWarning?Category=Furniture&amp;:size=600,400|vizlink)</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -2516,7 +2547,7 @@
         <v>&lt;p&gt;Hello Bob,&lt;/p&gt;&lt;p&gt;You have a low margin warning, please take a look this week&lt;/p&gt;VIZ_IMAGE(VizAlertsDemo/LowMarginWarning?Category=Office Supplies&amp;:size=600,400|vizlink)</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -2558,12 +2589,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>142</v>
       </c>
@@ -2589,7 +2620,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -2600,12 +2631,12 @@
         <v>152</v>
       </c>
       <c r="D2" s="1" t="str">
-        <f>"Test " &amp; B2 &amp; ": " &amp; C2</f>
+        <f t="shared" ref="D2:D10" si="0">"Test " &amp; B2 &amp; ": " &amp; C2</f>
         <v>Test 1: simple test</v>
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2616,12 +2647,12 @@
         <v>132</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f>"Test " &amp; B3 &amp; ": " &amp; C3</f>
+        <f t="shared" si="0"/>
         <v>Test 2: test for 2 numbers</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2632,11 +2663,11 @@
         <v>133</v>
       </c>
       <c r="D4" s="1" t="str">
-        <f>"Test " &amp; B4 &amp; ": " &amp; C4</f>
+        <f t="shared" si="0"/>
         <v>Test 3: number in x.xxx.xxx.xxxx format</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -2647,11 +2678,11 @@
         <v>134</v>
       </c>
       <c r="D5" s="1" t="str">
-        <f>"Test " &amp; B5 &amp; ": " &amp; C5</f>
+        <f t="shared" si="0"/>
         <v>Test 4: number in +x (xxx) xxx-xxxx format</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -2662,14 +2693,14 @@
         <v>135</v>
       </c>
       <c r="D6" s="1" t="str">
-        <f>"Test " &amp; B6 &amp; ": " &amp; C6</f>
+        <f t="shared" si="0"/>
         <v>Test 5: header in SMS</v>
       </c>
       <c r="G6" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -2680,14 +2711,14 @@
         <v>137</v>
       </c>
       <c r="D7" s="1" t="str">
-        <f>"Test " &amp; B7 &amp; ": " &amp; C7</f>
+        <f t="shared" si="0"/>
         <v>Test 6: footer in SMS</v>
       </c>
       <c r="H7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -2698,7 +2729,7 @@
         <v>139</v>
       </c>
       <c r="D8" s="1" t="str">
-        <f>"Test " &amp; B8 &amp; ": " &amp; C8</f>
+        <f t="shared" si="0"/>
         <v>Test 7: header and footer</v>
       </c>
       <c r="G8" t="s">
@@ -2708,7 +2739,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -2719,12 +2750,12 @@
         <v>159</v>
       </c>
       <c r="D9" s="1" t="str">
-        <f>"Test " &amp; B9 &amp; ": " &amp; C9</f>
+        <f t="shared" si="0"/>
         <v>Test 8: http://github.com/tableau/VizAlerts alert in body</v>
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -2735,11 +2766,11 @@
         <v>141</v>
       </c>
       <c r="D10" s="1" t="str">
-        <f>"Test " &amp; B10 &amp; ": " &amp; C10</f>
+        <f t="shared" si="0"/>
         <v>Test 9: VIZ_LINK() alert</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -2757,7 +2788,7 @@
         <v>Test 10: Consolidate 3 rows</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -2771,7 +2802,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -2804,9 +2835,9 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>142</v>
       </c>
@@ -2832,7 +2863,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -2847,7 +2878,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2865,7 +2896,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2883,7 +2914,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -2901,7 +2932,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -2919,7 +2950,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -2937,7 +2968,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -2955,7 +2986,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -2990,13 +3021,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>142</v>
       </c>
@@ -3013,7 +3044,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -3031,7 +3062,7 @@
         <v>12078319657</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Checking in initial changes for Issue #68: Implement smart default behavior for Advanced Alerts
</commit_message>
<xml_diff>
--- a/demo/tests.xlsx
+++ b/demo/tests.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcoles\Documents\GitHub\VizAlerts\demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mcoles\PycharmProjects\VizAlertsClean\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="2880" windowWidth="19275" windowHeight="11985" activeTab="1"/>
+    <workbookView xWindow="1440" yWindow="2880" windowWidth="19275" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Alerts" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="SMS Other Tests" sheetId="9" r:id="rId6"/>
     <sheet name="Excel Number Tests" sheetId="10" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -706,7 +706,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -741,7 +741,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -952,7 +952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1000,7 +1000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2585,9 +2585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2622,7 +2620,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -2638,7 +2636,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -2654,7 +2652,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -2669,7 +2667,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -2684,7 +2682,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -2702,7 +2700,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -2720,7 +2718,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -2741,7 +2739,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -2757,7 +2755,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -2772,7 +2770,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -2790,7 +2788,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="1">
         <v>10</v>
@@ -2804,7 +2802,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1">
         <v>10</v>
@@ -2832,7 +2830,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2865,7 +2863,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -2880,7 +2878,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -2898,7 +2896,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -2916,7 +2914,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -2934,7 +2932,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -2952,7 +2950,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -2970,7 +2968,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -2988,7 +2986,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -3021,9 +3019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3046,7 +3042,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -3064,7 +3060,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Updating user guide and VizAlertsDemo workbook.
</commit_message>
<xml_diff>
--- a/demo/tests.xlsx
+++ b/demo/tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="2880" windowWidth="19275" windowHeight="11985"/>
+    <workbookView xWindow="1440" yWindow="2880" windowWidth="19275" windowHeight="11985" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Alerts" sheetId="5" r:id="rId1"/>
@@ -952,7 +952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -2585,7 +2585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Fix for 2019.1 compatibility and a few other minor bugs / doc updates
</commit_message>
<xml_diff>
--- a/demo/tests.xlsx
+++ b/demo/tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="2880" windowWidth="19275" windowHeight="11985" activeTab="4"/>
+    <workbookView xWindow="1440" yWindow="2880" windowWidth="19275" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Alerts" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="183">
   <si>
     <t xml:space="preserve"> Email Action *</t>
   </si>
@@ -570,6 +570,15 @@
   </si>
   <si>
     <t>Multiple text links</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
   </si>
 </sst>
 </file>
@@ -631,11 +640,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -952,9 +963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1000,12 +1009,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="14" style="5" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.28515625" customWidth="1"/>
@@ -1021,7 +1033,7 @@
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1053,7 +1065,7 @@
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1075,7 +1087,7 @@
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1099,7 +1111,7 @@
       <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1123,7 +1135,7 @@
       <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1147,7 +1159,7 @@
       <c r="B6" s="1">
         <v>5</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1169,7 +1181,7 @@
       <c r="B7" s="1">
         <v>6</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1193,7 +1205,7 @@
       <c r="B8" s="1">
         <v>7</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1217,7 +1229,7 @@
       <c r="B9" s="1">
         <v>8</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1239,7 +1251,7 @@
       <c r="B10" s="1">
         <v>9</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1261,7 +1273,7 @@
       <c r="B11" s="1">
         <v>10</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1283,7 +1295,7 @@
       <c r="B12" s="1">
         <v>11</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
         <v>104</v>
       </c>
@@ -1305,7 +1317,7 @@
       <c r="B13" s="1">
         <v>12</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="1" t="s">
         <v>106</v>
       </c>
@@ -1327,7 +1339,7 @@
       <c r="B14" s="1">
         <v>13</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="1" t="s">
         <v>108</v>
       </c>
@@ -1349,7 +1361,7 @@
       <c r="B15" s="1">
         <v>14</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="1" t="s">
         <v>110</v>
       </c>
@@ -1371,7 +1383,7 @@
       <c r="B16" s="1">
         <v>15</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
         <v>112</v>
       </c>
@@ -1393,7 +1405,7 @@
       <c r="B17" s="1">
         <v>16</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1415,7 +1427,7 @@
       <c r="B18" s="1">
         <v>17</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1439,7 +1451,7 @@
       <c r="B19" s="1">
         <v>18</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1461,7 +1473,7 @@
       <c r="B20" s="1">
         <v>19</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="1" t="s">
         <v>29</v>
       </c>
@@ -1485,7 +1497,7 @@
       <c r="B21" s="1">
         <v>20</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="1" t="s">
         <v>32</v>
       </c>
@@ -1509,7 +1521,7 @@
       <c r="B22" s="1">
         <v>21</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="4"/>
       <c r="D22" s="1" t="s">
         <v>34</v>
       </c>
@@ -1531,7 +1543,7 @@
       <c r="B23" s="1">
         <v>22</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="4"/>
       <c r="D23" s="1" t="s">
         <v>38</v>
       </c>
@@ -1555,7 +1567,7 @@
       <c r="B24" s="1">
         <v>23</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" s="4"/>
       <c r="D24" s="1" t="s">
         <v>39</v>
       </c>
@@ -1579,7 +1591,7 @@
       <c r="B25" s="1">
         <v>24</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="C25" s="4"/>
       <c r="D25" s="1" t="s">
         <v>114</v>
       </c>
@@ -1606,8 +1618,8 @@
         <f>B25+1</f>
         <v>25</v>
       </c>
-      <c r="C26" s="1">
-        <v>1</v>
+      <c r="C26" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>4</v>
@@ -1632,8 +1644,8 @@
         <f>B26</f>
         <v>25</v>
       </c>
-      <c r="C27" s="1">
-        <v>2</v>
+      <c r="C27" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>4</v>
@@ -1658,8 +1670,8 @@
         <f>B26</f>
         <v>25</v>
       </c>
-      <c r="C28" s="1">
-        <v>3</v>
+      <c r="C28" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>4</v>
@@ -1684,8 +1696,8 @@
         <f>B26+1</f>
         <v>26</v>
       </c>
-      <c r="C29" s="1">
-        <v>1</v>
+      <c r="C29" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>13</v>
@@ -1710,8 +1722,8 @@
         <f>B29</f>
         <v>26</v>
       </c>
-      <c r="C30" s="1">
-        <v>2</v>
+      <c r="C30" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>13</v>
@@ -1736,8 +1748,8 @@
         <f>B29</f>
         <v>26</v>
       </c>
-      <c r="C31" s="1">
-        <v>3</v>
+      <c r="C31" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>13</v>
@@ -1762,8 +1774,8 @@
         <f>B29+1</f>
         <v>27</v>
       </c>
-      <c r="C32" s="1">
-        <v>1</v>
+      <c r="C32" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>14</v>
@@ -1788,8 +1800,8 @@
         <f>B32</f>
         <v>27</v>
       </c>
-      <c r="C33" s="1">
-        <v>2</v>
+      <c r="C33" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>14</v>
@@ -1814,8 +1826,8 @@
         <f>B32</f>
         <v>27</v>
       </c>
-      <c r="C34" s="1">
-        <v>3</v>
+      <c r="C34" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>14</v>
@@ -1840,8 +1852,8 @@
         <f>B32+1</f>
         <v>28</v>
       </c>
-      <c r="C35" s="1">
-        <v>1</v>
+      <c r="C35" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>36</v>
@@ -1866,8 +1878,8 @@
         <f>B35</f>
         <v>28</v>
       </c>
-      <c r="C36" s="1">
-        <v>2</v>
+      <c r="C36" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>36</v>
@@ -1892,8 +1904,8 @@
         <f>B35+1</f>
         <v>29</v>
       </c>
-      <c r="C37" s="1">
-        <v>1</v>
+      <c r="C37" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>58</v>
@@ -1920,8 +1932,8 @@
         <f>B37</f>
         <v>29</v>
       </c>
-      <c r="C38" s="1">
-        <v>2</v>
+      <c r="C38" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>58</v>
@@ -1946,8 +1958,8 @@
         <f>B37</f>
         <v>29</v>
       </c>
-      <c r="C39" s="1">
-        <v>3</v>
+      <c r="C39" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>58</v>
@@ -1972,8 +1984,8 @@
         <f>B37+1</f>
         <v>30</v>
       </c>
-      <c r="C40" s="1">
-        <v>1</v>
+      <c r="C40" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>37</v>
@@ -2000,8 +2012,8 @@
         <f>B40</f>
         <v>30</v>
       </c>
-      <c r="C41" s="1">
-        <v>2</v>
+      <c r="C41" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>37</v>
@@ -2026,8 +2038,8 @@
         <f>B40</f>
         <v>30</v>
       </c>
-      <c r="C42" s="1">
-        <v>3</v>
+      <c r="C42" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>37</v>
@@ -2052,8 +2064,8 @@
         <f>B40+1</f>
         <v>31</v>
       </c>
-      <c r="C43" s="1">
-        <v>1</v>
+      <c r="C43" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>62</v>
@@ -2080,8 +2092,8 @@
         <f>B43</f>
         <v>31</v>
       </c>
-      <c r="C44" s="1">
-        <v>2</v>
+      <c r="C44" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>62</v>
@@ -2106,8 +2118,8 @@
         <f>B43</f>
         <v>31</v>
       </c>
-      <c r="C45" s="1">
-        <v>3</v>
+      <c r="C45" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>62</v>
@@ -2131,8 +2143,8 @@
       <c r="B46">
         <v>32</v>
       </c>
-      <c r="C46" s="1">
-        <v>1</v>
+      <c r="C46" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>179</v>
@@ -2149,6 +2161,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2585,7 +2598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>